<commit_message>
commented clearing form inputs when adding lecture
</commit_message>
<xml_diff>
--- a/web/room_excel_template.xlsx
+++ b/web/room_excel_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Programming\Object Oriented Programming\SmartCampus\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Programming\Object Oriented Programming\Final\SmartCampus\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,49 +24,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>room_name</t>
+    <t>ტიპი</t>
   </si>
   <si>
-    <t>ოთახის ნომერი</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo Bold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ოთახის</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> N</t>
+    </r>
   </si>
   <si>
-    <t>room_floor</t>
-  </si>
-  <si>
-    <t>სართული</t>
-  </si>
-  <si>
-    <t>ადგილების რაოდენობა</t>
-  </si>
-  <si>
-    <t>capacity</t>
-  </si>
-  <si>
-    <t>room_type</t>
-  </si>
-  <si>
-    <t>შეიყვანეთ რიცხვი(აუდიტორია: 1, სხვა:2)</t>
-  </si>
-  <si>
-    <t>seat_type</t>
-  </si>
-  <si>
-    <t>შეიყვანეთ რიცხვი(სკამები და მერხები: 1, სკამ-მერხები (ხის): 2, სკამ-მერხები (პლასტმასის):3, მაგიდები: 4, კომპიუტერები: 5)</t>
-  </si>
-  <si>
-    <t>can_be_booked</t>
-  </si>
-  <si>
-    <t>შეიყვანეთ რიცხვი(კი: 1, არა: 0)</t>
+    <t>სტუდ. ტევადობა</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +75,12 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo Bold"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,59 +454,31 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="6" width="19" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
     </row>
   </sheetData>

</xml_diff>